<commit_message>
Reexport csv tabs for BGBSC
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/BGBSC/BAU Global Battery Storage Cap.xlsx
+++ b/InputData/endo-learn/BGBSC/BAU Global Battery Storage Cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\endo-learn\BGBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\endo-learn\BGBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{008D9D4E-A250-406B-A4A4-9DDC8AD5605F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F003864B-0DEB-4A0F-AD2C-48D451586C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="EV Batteries" sheetId="5" r:id="rId3"/>
     <sheet name="EV Sigmoid Fitting" sheetId="10" r:id="rId4"/>
     <sheet name="Calculations" sheetId="7" r:id="rId5"/>
-    <sheet name="BGBSC" sheetId="6" r:id="rId6"/>
+    <sheet name="SYGBSC" sheetId="11" r:id="rId6"/>
+    <sheet name="BGBSC" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="ec_50">'EV Sigmoid Fitting'!$B$4</definedName>
@@ -59,7 +60,7 @@
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>BGBSC BAU Global Battery Storage Capacity</t>
   </si>
@@ -665,7 +666,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'[2]EV Batteries'!$B$9:$Y$9</c:f>
+              <c:f>'[1]EV Batteries'!$B$9:$Y$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -746,7 +747,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[2]EV Batteries'!$B$13:$Y$13</c:f>
+              <c:f>'[1]EV Batteries'!$B$13:$Y$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1020,7 +1021,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$G$1</c:f>
+              <c:f>[2]Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1053,7 +1054,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$F$2:$F$35</c:f>
+              <c:f>[2]Sheet1!$F$2:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1158,7 +1159,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$G$2:$G$35</c:f>
+              <c:f>[2]Sheet1!$G$2:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1243,7 +1244,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$H$1</c:f>
+              <c:f>[2]Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1276,7 +1277,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$F$2:$F$35</c:f>
+              <c:f>[2]Sheet1!$F$2:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1381,7 +1382,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$H$2:$H$35</c:f>
+              <c:f>[2]Sheet1!$H$2:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1764,7 +1765,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$G$1</c:f>
+              <c:f>[2]Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1797,7 +1798,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$F$2:$F$35</c:f>
+              <c:f>[2]Sheet1!$F$2:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1902,7 +1903,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$G$2:$G$35</c:f>
+              <c:f>[2]Sheet1!$G$2:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1987,7 +1988,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$H$1</c:f>
+              <c:f>[2]Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2020,7 +2021,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$F$2:$F$35</c:f>
+              <c:f>[2]Sheet1!$F$2:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2125,7 +2126,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$H$2:$H$35</c:f>
+              <c:f>[2]Sheet1!$H$2:$H$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -2538,7 +2539,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[2]Calculations!$A$12</c:f>
+              <c:f>[1]Calculations!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2573,7 +2574,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[2]Calculations!$B$11:$AG$11</c:f>
+              <c:f>[1]Calculations!$B$11:$AG$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2678,7 +2679,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[2]Calculations!$B$12:$AG$12</c:f>
+              <c:f>[1]Calculations!$B$12:$AG$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2733,7 +2734,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[2]Calculations!$A$13</c:f>
+              <c:f>[1]Calculations!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2768,7 +2769,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[2]Calculations!$B$11:$AG$11</c:f>
+              <c:f>[1]Calculations!$B$11:$AG$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2873,7 +2874,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[2]Calculations!$B$13:$AK$13</c:f>
+              <c:f>[1]Calculations!$B$13:$AK$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -2922,7 +2923,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>[2]Calculations!$A$14</c:f>
+              <c:f>[1]Calculations!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2957,7 +2958,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[2]Calculations!$B$11:$AG$11</c:f>
+              <c:f>[1]Calculations!$B$11:$AG$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -3062,7 +3063,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[2]Calculations!$B$14:$AK$14</c:f>
+              <c:f>[1]Calculations!$B$14:$AK$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -3374,7 +3375,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[2]Calculations!$A$17</c:f>
+              <c:f>[1]Calculations!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3409,7 +3410,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[2]Calculations!$C$16:$AH$16</c:f>
+              <c:f>[1]Calculations!$C$16:$AH$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -3514,7 +3515,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[2]Calculations!$C$17:$AH$17</c:f>
+              <c:f>[1]Calculations!$C$17:$AH$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -7139,350 +7140,6 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="G1" t="str">
-            <v>y</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>ycalc</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="F2">
-            <v>2019</v>
-          </cell>
-          <cell r="G2">
-            <v>2375000</v>
-          </cell>
-          <cell r="H2">
-            <v>1389132.164056371</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="F3">
-            <v>2020</v>
-          </cell>
-          <cell r="G3">
-            <v>1750000</v>
-          </cell>
-          <cell r="H3">
-            <v>2021843.2718926258</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="F4">
-            <v>2021</v>
-          </cell>
-          <cell r="G4">
-            <v>2500000</v>
-          </cell>
-          <cell r="H4">
-            <v>2835096.85528416</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="F5">
-            <v>2022</v>
-          </cell>
-          <cell r="G5">
-            <v>3875000</v>
-          </cell>
-          <cell r="H5">
-            <v>3872186.6405841364</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="F6">
-            <v>2023</v>
-          </cell>
-          <cell r="G6">
-            <v>5375000</v>
-          </cell>
-          <cell r="H6">
-            <v>5181480.7302558515</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="F7">
-            <v>2024</v>
-          </cell>
-          <cell r="G7">
-            <v>7000000</v>
-          </cell>
-          <cell r="H7">
-            <v>6813588.8256108928</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="F8">
-            <v>2025</v>
-          </cell>
-          <cell r="G8">
-            <v>8500000</v>
-          </cell>
-          <cell r="H8">
-            <v>8816233.2840826623</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="F9">
-            <v>2026</v>
-          </cell>
-          <cell r="G9">
-            <v>10375000</v>
-          </cell>
-          <cell r="H9">
-            <v>11226473.258701244</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="F10">
-            <v>2027</v>
-          </cell>
-          <cell r="G10">
-            <v>13625000</v>
-          </cell>
-          <cell r="H10">
-            <v>14060660.844756193</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="F11">
-            <v>2028</v>
-          </cell>
-          <cell r="G11">
-            <v>17125000</v>
-          </cell>
-          <cell r="H11">
-            <v>17303745.690459114</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="F12">
-            <v>2029</v>
-          </cell>
-          <cell r="G12">
-            <v>21000000</v>
-          </cell>
-          <cell r="H12">
-            <v>20900972.172630183</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="F13">
-            <v>2030</v>
-          </cell>
-          <cell r="G13">
-            <v>25500000</v>
-          </cell>
-          <cell r="H13">
-            <v>24755807.045043826</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="F14">
-            <v>2031</v>
-          </cell>
-          <cell r="G14">
-            <v>29250000</v>
-          </cell>
-          <cell r="H14">
-            <v>28737059.300076034</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="F15">
-            <v>2032</v>
-          </cell>
-          <cell r="G15">
-            <v>33375000</v>
-          </cell>
-          <cell r="H15">
-            <v>32695224.467196576</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="F16">
-            <v>2033</v>
-          </cell>
-          <cell r="G16">
-            <v>36625000</v>
-          </cell>
-          <cell r="H16">
-            <v>36484206.532142162</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="F17">
-            <v>2034</v>
-          </cell>
-          <cell r="G17">
-            <v>39750000</v>
-          </cell>
-          <cell r="H17">
-            <v>39982014.338317864</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="F18">
-            <v>2035</v>
-          </cell>
-          <cell r="G18">
-            <v>42625000</v>
-          </cell>
-          <cell r="H18">
-            <v>43104531.090709515</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="F19">
-            <v>2036</v>
-          </cell>
-          <cell r="G19">
-            <v>45250000</v>
-          </cell>
-          <cell r="H19">
-            <v>45809663.601785377</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="F20">
-            <v>2037</v>
-          </cell>
-          <cell r="G20">
-            <v>47375000</v>
-          </cell>
-          <cell r="H20">
-            <v>48092978.656097099</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="F21">
-            <v>2038</v>
-          </cell>
-          <cell r="G21">
-            <v>49375000</v>
-          </cell>
-          <cell r="H21">
-            <v>49978278.595441304</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="F22">
-            <v>2039</v>
-          </cell>
-          <cell r="G22">
-            <v>51625000</v>
-          </cell>
-          <cell r="H22">
-            <v>51506844.678802423</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="F23">
-            <v>2040</v>
-          </cell>
-          <cell r="G23">
-            <v>54125000</v>
-          </cell>
-          <cell r="H23">
-            <v>52727977.781544022</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="F24">
-            <v>2041</v>
-          </cell>
-          <cell r="H24">
-            <v>53692031.914074436</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="F25">
-            <v>2042</v>
-          </cell>
-          <cell r="H25">
-            <v>54446041.034588695</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="F26">
-            <v>2043</v>
-          </cell>
-          <cell r="H26">
-            <v>55031465.127539933</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="F27">
-            <v>2044</v>
-          </cell>
-          <cell r="H27">
-            <v>55483417.471983574</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="F28">
-            <v>2045</v>
-          </cell>
-          <cell r="H28">
-            <v>55830797.702772141</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="F29">
-            <v>2046</v>
-          </cell>
-          <cell r="H29">
-            <v>56096900.262841031</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="F30">
-            <v>2047</v>
-          </cell>
-          <cell r="H30">
-            <v>56300214.433481641</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="F31">
-            <v>2048</v>
-          </cell>
-          <cell r="H31">
-            <v>56455248.150785372</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="F32">
-            <v>2049</v>
-          </cell>
-          <cell r="H32">
-            <v>56573288.007629298</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="F33">
-            <v>2050</v>
-          </cell>
-          <cell r="H33">
-            <v>56663058.09199407</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
@@ -8251,6 +7908,350 @@
       <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7" refreshError="1"/>
       <sheetData sheetId="8" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="G1" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>ycalc</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="F2">
+            <v>2019</v>
+          </cell>
+          <cell r="G2">
+            <v>2375000</v>
+          </cell>
+          <cell r="H2">
+            <v>1389132.164056371</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="F3">
+            <v>2020</v>
+          </cell>
+          <cell r="G3">
+            <v>1750000</v>
+          </cell>
+          <cell r="H3">
+            <v>2021843.2718926258</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="F4">
+            <v>2021</v>
+          </cell>
+          <cell r="G4">
+            <v>2500000</v>
+          </cell>
+          <cell r="H4">
+            <v>2835096.85528416</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="F5">
+            <v>2022</v>
+          </cell>
+          <cell r="G5">
+            <v>3875000</v>
+          </cell>
+          <cell r="H5">
+            <v>3872186.6405841364</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="F6">
+            <v>2023</v>
+          </cell>
+          <cell r="G6">
+            <v>5375000</v>
+          </cell>
+          <cell r="H6">
+            <v>5181480.7302558515</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="F7">
+            <v>2024</v>
+          </cell>
+          <cell r="G7">
+            <v>7000000</v>
+          </cell>
+          <cell r="H7">
+            <v>6813588.8256108928</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="F8">
+            <v>2025</v>
+          </cell>
+          <cell r="G8">
+            <v>8500000</v>
+          </cell>
+          <cell r="H8">
+            <v>8816233.2840826623</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="F9">
+            <v>2026</v>
+          </cell>
+          <cell r="G9">
+            <v>10375000</v>
+          </cell>
+          <cell r="H9">
+            <v>11226473.258701244</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="F10">
+            <v>2027</v>
+          </cell>
+          <cell r="G10">
+            <v>13625000</v>
+          </cell>
+          <cell r="H10">
+            <v>14060660.844756193</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="F11">
+            <v>2028</v>
+          </cell>
+          <cell r="G11">
+            <v>17125000</v>
+          </cell>
+          <cell r="H11">
+            <v>17303745.690459114</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="F12">
+            <v>2029</v>
+          </cell>
+          <cell r="G12">
+            <v>21000000</v>
+          </cell>
+          <cell r="H12">
+            <v>20900972.172630183</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="F13">
+            <v>2030</v>
+          </cell>
+          <cell r="G13">
+            <v>25500000</v>
+          </cell>
+          <cell r="H13">
+            <v>24755807.045043826</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="F14">
+            <v>2031</v>
+          </cell>
+          <cell r="G14">
+            <v>29250000</v>
+          </cell>
+          <cell r="H14">
+            <v>28737059.300076034</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="F15">
+            <v>2032</v>
+          </cell>
+          <cell r="G15">
+            <v>33375000</v>
+          </cell>
+          <cell r="H15">
+            <v>32695224.467196576</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="F16">
+            <v>2033</v>
+          </cell>
+          <cell r="G16">
+            <v>36625000</v>
+          </cell>
+          <cell r="H16">
+            <v>36484206.532142162</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="F17">
+            <v>2034</v>
+          </cell>
+          <cell r="G17">
+            <v>39750000</v>
+          </cell>
+          <cell r="H17">
+            <v>39982014.338317864</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="F18">
+            <v>2035</v>
+          </cell>
+          <cell r="G18">
+            <v>42625000</v>
+          </cell>
+          <cell r="H18">
+            <v>43104531.090709515</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="F19">
+            <v>2036</v>
+          </cell>
+          <cell r="G19">
+            <v>45250000</v>
+          </cell>
+          <cell r="H19">
+            <v>45809663.601785377</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="F20">
+            <v>2037</v>
+          </cell>
+          <cell r="G20">
+            <v>47375000</v>
+          </cell>
+          <cell r="H20">
+            <v>48092978.656097099</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="F21">
+            <v>2038</v>
+          </cell>
+          <cell r="G21">
+            <v>49375000</v>
+          </cell>
+          <cell r="H21">
+            <v>49978278.595441304</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="F22">
+            <v>2039</v>
+          </cell>
+          <cell r="G22">
+            <v>51625000</v>
+          </cell>
+          <cell r="H22">
+            <v>51506844.678802423</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="F23">
+            <v>2040</v>
+          </cell>
+          <cell r="G23">
+            <v>54125000</v>
+          </cell>
+          <cell r="H23">
+            <v>52727977.781544022</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="F24">
+            <v>2041</v>
+          </cell>
+          <cell r="H24">
+            <v>53692031.914074436</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="F25">
+            <v>2042</v>
+          </cell>
+          <cell r="H25">
+            <v>54446041.034588695</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="F26">
+            <v>2043</v>
+          </cell>
+          <cell r="H26">
+            <v>55031465.127539933</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="F27">
+            <v>2044</v>
+          </cell>
+          <cell r="H27">
+            <v>55483417.471983574</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="F28">
+            <v>2045</v>
+          </cell>
+          <cell r="H28">
+            <v>55830797.702772141</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="F29">
+            <v>2046</v>
+          </cell>
+          <cell r="H29">
+            <v>56096900.262841031</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="F30">
+            <v>2047</v>
+          </cell>
+          <cell r="H30">
+            <v>56300214.433481641</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="F31">
+            <v>2048</v>
+          </cell>
+          <cell r="H31">
+            <v>56455248.150785372</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="F32">
+            <v>2049</v>
+          </cell>
+          <cell r="H32">
+            <v>56573288.007629298</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="F33">
+            <v>2050</v>
+          </cell>
+          <cell r="H33">
+            <v>56663058.09199407</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10712,131 +10713,131 @@
         <v>21</v>
       </c>
       <c r="B6" s="13">
-        <f>'[2]Grid Battery Storage'!B6</f>
+        <f>'[1]Grid Battery Storage'!B6</f>
         <v>23809.523809523806</v>
       </c>
       <c r="C6">
-        <f>TREND('[2]Grid Battery Storage'!$B$6:$C$6,'[2]Grid Battery Storage'!$B$4:$C$4,'[2]Grid Battery Storage'!C8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$B$6:$C$6,'[1]Grid Battery Storage'!$B$4:$C$4,'[1]Grid Battery Storage'!C8)</f>
         <v>23809.52380952239</v>
       </c>
       <c r="D6">
-        <f>TREND('[2]Grid Battery Storage'!$B$6:$C$6,'[2]Grid Battery Storage'!$B$4:$C$4,'[2]Grid Battery Storage'!D8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$B$6:$C$6,'[1]Grid Battery Storage'!$B$4:$C$4,'[1]Grid Battery Storage'!D8)</f>
         <v>50000</v>
       </c>
       <c r="E6">
-        <f>TREND('[2]Grid Battery Storage'!$B$6:$C$6,'[2]Grid Battery Storage'!$B$4:$C$4,'[2]Grid Battery Storage'!E8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$B$6:$C$6,'[1]Grid Battery Storage'!$B$4:$C$4,'[1]Grid Battery Storage'!E8)</f>
         <v>76190.47619047761</v>
       </c>
       <c r="F6">
-        <f>TREND('[2]Grid Battery Storage'!$B$6:$C$6,'[2]Grid Battery Storage'!$B$4:$C$4,'[2]Grid Battery Storage'!F8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$B$6:$C$6,'[1]Grid Battery Storage'!$B$4:$C$4,'[1]Grid Battery Storage'!F8)</f>
         <v>102380.95238095522</v>
       </c>
       <c r="G6">
-        <f>TREND('[2]Grid Battery Storage'!$B$6:$C$6,'[2]Grid Battery Storage'!$B$4:$C$4,'[2]Grid Battery Storage'!G8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$B$6:$C$6,'[1]Grid Battery Storage'!$B$4:$C$4,'[1]Grid Battery Storage'!G8)</f>
         <v>128571.42857143283</v>
       </c>
       <c r="H6">
-        <f>TREND('[2]Grid Battery Storage'!$B$6:$C$6,'[2]Grid Battery Storage'!$B$4:$C$4,'[2]Grid Battery Storage'!H8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$B$6:$C$6,'[1]Grid Battery Storage'!$B$4:$C$4,'[1]Grid Battery Storage'!H8)</f>
         <v>154761.90476190299</v>
       </c>
       <c r="I6">
-        <f>TREND('[2]Grid Battery Storage'!$C$6:$D$6,'[2]Grid Battery Storage'!$C$4:$D$4,'[2]Grid Battery Storage'!I8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$C$6:$D$6,'[1]Grid Battery Storage'!$C$4:$D$4,'[1]Grid Battery Storage'!I8)</f>
         <v>238095.2380952239</v>
       </c>
       <c r="J6">
-        <f>TREND('[2]Grid Battery Storage'!$C$6:$D$6,'[2]Grid Battery Storage'!$C$4:$D$4,'[2]Grid Battery Storage'!J8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$C$6:$D$6,'[1]Grid Battery Storage'!$C$4:$D$4,'[1]Grid Battery Storage'!J8)</f>
         <v>321428.57142856717</v>
       </c>
       <c r="K6">
-        <f>TREND('[2]Grid Battery Storage'!$C$6:$D$6,'[2]Grid Battery Storage'!$C$4:$D$4,'[2]Grid Battery Storage'!K8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$C$6:$D$6,'[1]Grid Battery Storage'!$C$4:$D$4,'[1]Grid Battery Storage'!K8)</f>
         <v>404761.90476191044</v>
       </c>
       <c r="L6">
-        <f>TREND('[2]Grid Battery Storage'!$C$6:$D$6,'[2]Grid Battery Storage'!$C$4:$D$4,'[2]Grid Battery Storage'!L8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$C$6:$D$6,'[1]Grid Battery Storage'!$C$4:$D$4,'[1]Grid Battery Storage'!L8)</f>
         <v>488095.2380952239</v>
       </c>
       <c r="M6">
-        <f>TREND('[2]Grid Battery Storage'!$C$6:$D$6,'[2]Grid Battery Storage'!$C$4:$D$4,'[2]Grid Battery Storage'!M8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$C$6:$D$6,'[1]Grid Battery Storage'!$C$4:$D$4,'[1]Grid Battery Storage'!M8)</f>
         <v>571428.57142856717</v>
       </c>
       <c r="N6">
-        <f>TREND('[2]Grid Battery Storage'!$D$6:$E$6,'[2]Grid Battery Storage'!$D$4:$E$4,'[2]Grid Battery Storage'!N8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$D$6:$E$6,'[1]Grid Battery Storage'!$D$4:$E$4,'[1]Grid Battery Storage'!N8)</f>
         <v>685714.28571429849</v>
       </c>
       <c r="O6">
-        <f>TREND('[2]Grid Battery Storage'!$D$6:$E$6,'[2]Grid Battery Storage'!$D$4:$E$4,'[2]Grid Battery Storage'!O8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$D$6:$E$6,'[1]Grid Battery Storage'!$D$4:$E$4,'[1]Grid Battery Storage'!O8)</f>
         <v>800000</v>
       </c>
       <c r="P6">
-        <f>TREND('[2]Grid Battery Storage'!$D$6:$E$6,'[2]Grid Battery Storage'!$D$4:$E$4,'[2]Grid Battery Storage'!P8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$D$6:$E$6,'[1]Grid Battery Storage'!$D$4:$E$4,'[1]Grid Battery Storage'!P8)</f>
         <v>914285.71428573132</v>
       </c>
       <c r="Q6">
-        <f>TREND('[2]Grid Battery Storage'!$D$6:$E$6,'[2]Grid Battery Storage'!$D$4:$E$4,'[2]Grid Battery Storage'!Q8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$D$6:$E$6,'[1]Grid Battery Storage'!$D$4:$E$4,'[1]Grid Battery Storage'!Q8)</f>
         <v>1028571.4285714328</v>
       </c>
       <c r="R6">
-        <f>TREND('[2]Grid Battery Storage'!$D$6:$E$6,'[2]Grid Battery Storage'!$D$4:$E$4,'[2]Grid Battery Storage'!R8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$D$6:$E$6,'[1]Grid Battery Storage'!$D$4:$E$4,'[1]Grid Battery Storage'!R8)</f>
         <v>1142857.1428571343</v>
       </c>
       <c r="S6">
-        <f>TREND('[2]Grid Battery Storage'!$E$6:$F$6,'[2]Grid Battery Storage'!$E$4:$F$4,'[2]Grid Battery Storage'!S8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$E$6:$F$6,'[1]Grid Battery Storage'!$E$4:$F$4,'[1]Grid Battery Storage'!S8)</f>
         <v>1319047.6190475821</v>
       </c>
       <c r="T6">
-        <f>TREND('[2]Grid Battery Storage'!$E$6:$F$6,'[2]Grid Battery Storage'!$E$4:$F$4,'[2]Grid Battery Storage'!T8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$E$6:$F$6,'[1]Grid Battery Storage'!$E$4:$F$4,'[1]Grid Battery Storage'!T8)</f>
         <v>1495238.0952380896</v>
       </c>
       <c r="U6">
-        <f>TREND('[2]Grid Battery Storage'!$E$6:$F$6,'[2]Grid Battery Storage'!$E$4:$F$4,'[2]Grid Battery Storage'!U8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$E$6:$F$6,'[1]Grid Battery Storage'!$E$4:$F$4,'[1]Grid Battery Storage'!U8)</f>
         <v>1671428.5714285374</v>
       </c>
       <c r="V6">
-        <f>TREND('[2]Grid Battery Storage'!$E$6:$F$6,'[2]Grid Battery Storage'!$E$4:$F$4,'[2]Grid Battery Storage'!V8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$E$6:$F$6,'[1]Grid Battery Storage'!$E$4:$F$4,'[1]Grid Battery Storage'!V8)</f>
         <v>1847619.0476190448</v>
       </c>
       <c r="W6">
-        <f>TREND('[2]Grid Battery Storage'!$E$6:$F$6,'[2]Grid Battery Storage'!$E$4:$F$4,'[2]Grid Battery Storage'!W8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$E$6:$F$6,'[1]Grid Battery Storage'!$E$4:$F$4,'[1]Grid Battery Storage'!W8)</f>
         <v>2023809.5238094926</v>
       </c>
       <c r="X6">
-        <f>TREND('[2]Grid Battery Storage'!$F$6:$G$6,'[2]Grid Battery Storage'!$F$4:$G$4,'[2]Grid Battery Storage'!X8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$F$6:$G$6,'[1]Grid Battery Storage'!$F$4:$G$4,'[1]Grid Battery Storage'!X8)</f>
         <v>2261904.7619047761</v>
       </c>
       <c r="Y6">
-        <f>TREND('[2]Grid Battery Storage'!$F$6:$G$6,'[2]Grid Battery Storage'!$F$4:$G$4,'[2]Grid Battery Storage'!Y8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$F$6:$G$6,'[1]Grid Battery Storage'!$F$4:$G$4,'[1]Grid Battery Storage'!Y8)</f>
         <v>2500000.0000000596</v>
       </c>
       <c r="Z6">
-        <f>TREND('[2]Grid Battery Storage'!$F$6:$G$6,'[2]Grid Battery Storage'!$F$4:$G$4,'[2]Grid Battery Storage'!Z8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$F$6:$G$6,'[1]Grid Battery Storage'!$F$4:$G$4,'[1]Grid Battery Storage'!Z8)</f>
         <v>2738095.2380952835</v>
       </c>
       <c r="AA6">
-        <f>TREND('[2]Grid Battery Storage'!$F$6:$G$6,'[2]Grid Battery Storage'!$F$4:$G$4,'[2]Grid Battery Storage'!AA8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$F$6:$G$6,'[1]Grid Battery Storage'!$F$4:$G$4,'[1]Grid Battery Storage'!AA8)</f>
         <v>2976190.4761905074</v>
       </c>
       <c r="AB6">
-        <f>TREND('[2]Grid Battery Storage'!$F$6:$G$6,'[2]Grid Battery Storage'!$F$4:$G$4,'[2]Grid Battery Storage'!AB8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$F$6:$G$6,'[1]Grid Battery Storage'!$F$4:$G$4,'[1]Grid Battery Storage'!AB8)</f>
         <v>3214285.7142857313</v>
       </c>
       <c r="AC6">
-        <f>TREND('[2]Grid Battery Storage'!$G$6:$H$6,'[2]Grid Battery Storage'!$G$4:$H$4,'[2]Grid Battery Storage'!AC8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$G$6:$H$6,'[1]Grid Battery Storage'!$G$4:$H$4,'[1]Grid Battery Storage'!AC8)</f>
         <v>3440476.1904761791</v>
       </c>
       <c r="AD6">
-        <f>TREND('[2]Grid Battery Storage'!$G$6:$H$6,'[2]Grid Battery Storage'!$G$4:$H$4,'[2]Grid Battery Storage'!AD8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$G$6:$H$6,'[1]Grid Battery Storage'!$G$4:$H$4,'[1]Grid Battery Storage'!AD8)</f>
         <v>3666666.6666666865</v>
       </c>
       <c r="AE6">
-        <f>TREND('[2]Grid Battery Storage'!$G$6:$H$6,'[2]Grid Battery Storage'!$G$4:$H$4,'[2]Grid Battery Storage'!AE8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$G$6:$H$6,'[1]Grid Battery Storage'!$G$4:$H$4,'[1]Grid Battery Storage'!AE8)</f>
         <v>3892857.1428571343</v>
       </c>
       <c r="AF6">
-        <f>TREND('[2]Grid Battery Storage'!$G$6:$H$6,'[2]Grid Battery Storage'!$G$4:$H$4,'[2]Grid Battery Storage'!AF8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$G$6:$H$6,'[1]Grid Battery Storage'!$G$4:$H$4,'[1]Grid Battery Storage'!AF8)</f>
         <v>4119047.6190475821</v>
       </c>
       <c r="AG6">
-        <f>TREND('[2]Grid Battery Storage'!$G$6:$H$6,'[2]Grid Battery Storage'!$G$4:$H$4,'[2]Grid Battery Storage'!AG8)</f>
+        <f>TREND('[1]Grid Battery Storage'!$G$6:$H$6,'[1]Grid Battery Storage'!$G$4:$H$4,'[1]Grid Battery Storage'!AG8)</f>
         <v>4345238.0952380896</v>
       </c>
     </row>
@@ -10953,51 +10954,51 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <f>('[2]EV Batteries'!D10)*(1000)</f>
+        <f>('[1]EV Batteries'!D10)*(1000)</f>
         <v>230000</v>
       </c>
       <c r="C12">
-        <f>('[2]EV Batteries'!E10)*(1000)</f>
+        <f>('[1]EV Batteries'!E10)*(1000)</f>
         <v>490909.09090909094</v>
       </c>
       <c r="D12">
-        <f>('[2]EV Batteries'!F10)*(1000)</f>
+        <f>('[1]EV Batteries'!F10)*(1000)</f>
         <v>751818.18181818188</v>
       </c>
       <c r="E12">
-        <f>('[2]EV Batteries'!G10)*(1000)</f>
+        <f>('[1]EV Batteries'!G10)*(1000)</f>
         <v>1012727.2727272727</v>
       </c>
       <c r="F12">
-        <f>('[2]EV Batteries'!H10)*(1000)</f>
+        <f>('[1]EV Batteries'!H10)*(1000)</f>
         <v>1273636.3636363638</v>
       </c>
       <c r="G12">
-        <f>('[2]EV Batteries'!I10)*(1000)</f>
+        <f>('[1]EV Batteries'!I10)*(1000)</f>
         <v>1534545.4545454548</v>
       </c>
       <c r="H12">
-        <f>('[2]EV Batteries'!J10)*(1000)</f>
+        <f>('[1]EV Batteries'!J10)*(1000)</f>
         <v>1795454.5454545456</v>
       </c>
       <c r="I12">
-        <f>('[2]EV Batteries'!K10)*(1000)</f>
+        <f>('[1]EV Batteries'!K10)*(1000)</f>
         <v>2056363.6363636365</v>
       </c>
       <c r="J12">
-        <f>('[2]EV Batteries'!L10)*(1000)</f>
+        <f>('[1]EV Batteries'!L10)*(1000)</f>
         <v>2317272.7272727275</v>
       </c>
       <c r="K12">
-        <f>('[2]EV Batteries'!M10)*(1000)</f>
+        <f>('[1]EV Batteries'!M10)*(1000)</f>
         <v>2578181.8181818184</v>
       </c>
       <c r="L12">
-        <f>('[2]EV Batteries'!N10)*(1000)</f>
+        <f>('[1]EV Batteries'!N10)*(1000)</f>
         <v>2839090.9090909096</v>
       </c>
       <c r="M12">
-        <f>('[2]EV Batteries'!O10)*(1000)</f>
+        <f>('[1]EV Batteries'!O10)*(1000)</f>
         <v>3100000</v>
       </c>
     </row>
@@ -11006,43 +11007,43 @@
         <v>9</v>
       </c>
       <c r="N13">
-        <f>('[2]EV Batteries'!P10)*(1000)</f>
+        <f>('[1]EV Batteries'!P10)*(1000)</f>
         <v>3424790.5975175635</v>
       </c>
       <c r="O13">
-        <f>('[2]EV Batteries'!Q10)*(1000)</f>
+        <f>('[1]EV Batteries'!Q10)*(1000)</f>
         <v>3746501.3723235992</v>
       </c>
       <c r="P13">
-        <f>('[2]EV Batteries'!R10)*(1000)</f>
+        <f>('[1]EV Batteries'!R10)*(1000)</f>
         <v>4059905.3441759855</v>
       </c>
       <c r="Q13">
-        <f>('[2]EV Batteries'!S10)*(1000)</f>
+        <f>('[1]EV Batteries'!S10)*(1000)</f>
         <v>4360313.8003408825</v>
       </c>
       <c r="R13">
-        <f>('[2]EV Batteries'!T10)*(1000)</f>
+        <f>('[1]EV Batteries'!T10)*(1000)</f>
         <v>4643834.5503812227</v>
       </c>
       <c r="S13">
-        <f>('[2]EV Batteries'!U10)*(1000)</f>
+        <f>('[1]EV Batteries'!U10)*(1000)</f>
         <v>4907531.6444603689</v>
       </c>
       <c r="T13">
-        <f>('[2]EV Batteries'!V10)*(1000)</f>
+        <f>('[1]EV Batteries'!V10)*(1000)</f>
         <v>5149479.4152991604</v>
       </c>
       <c r="U13">
-        <f>('[2]EV Batteries'!W10)*(1000)</f>
+        <f>('[1]EV Batteries'!W10)*(1000)</f>
         <v>5368721.7605243968</v>
       </c>
       <c r="V13">
-        <f>('[2]EV Batteries'!X10)*(1000)</f>
+        <f>('[1]EV Batteries'!X10)*(1000)</f>
         <v>5565159.8514983393</v>
       </c>
       <c r="W13">
-        <f>('[2]EV Batteries'!Y10)*(1000)</f>
+        <f>('[1]EV Batteries'!Y10)*(1000)</f>
         <v>5739396.454520884</v>
       </c>
     </row>
@@ -11051,43 +11052,43 @@
         <v>10</v>
       </c>
       <c r="X14">
-        <f>('[2]EV Batteries'!Z10)*(1000)</f>
+        <f>('[1]EV Batteries'!Z10)*(1000)</f>
         <v>5892563.6833218094</v>
       </c>
       <c r="Y14">
-        <f>('[2]EV Batteries'!AA10)*(1000)</f>
+        <f>('[1]EV Batteries'!AA10)*(1000)</f>
         <v>6026155.5256387582</v>
       </c>
       <c r="Z14">
-        <f>('[2]EV Batteries'!AB10)*(1000)</f>
+        <f>('[1]EV Batteries'!AB10)*(1000)</f>
         <v>6141879.3779363325</v>
       </c>
       <c r="AA14">
-        <f>('[2]EV Batteries'!AC10)*(1000)</f>
+        <f>('[1]EV Batteries'!AC10)*(1000)</f>
         <v>6241534.0085637206</v>
       </c>
       <c r="AB14">
-        <f>('[2]EV Batteries'!AD10)*(1000)</f>
+        <f>('[1]EV Batteries'!AD10)*(1000)</f>
         <v>6326915.950859325</v>
       </c>
       <c r="AC14">
-        <f>('[2]EV Batteries'!AE10)*(1000)</f>
+        <f>('[1]EV Batteries'!AE10)*(1000)</f>
         <v>6399752.6614421792</v>
       </c>
       <c r="AD14">
-        <f>('[2]EV Batteries'!AF10)*(1000)</f>
+        <f>('[1]EV Batteries'!AF10)*(1000)</f>
         <v>6461658.7298551602</v>
       </c>
       <c r="AE14">
-        <f>('[2]EV Batteries'!AG10)*(1000)</f>
+        <f>('[1]EV Batteries'!AG10)*(1000)</f>
         <v>6514110.623151809</v>
       </c>
       <c r="AF14">
-        <f>('[2]EV Batteries'!AH10)*(1000)</f>
+        <f>('[1]EV Batteries'!AH10)*(1000)</f>
         <v>6558435.4749555839</v>
       </c>
       <c r="AG14">
-        <f>('[2]EV Batteries'!AI10)*(1000)</f>
+        <f>('[1]EV Batteries'!AI10)*(1000)</f>
         <v>6595809.921999068</v>
       </c>
     </row>
@@ -11345,251 +11346,273 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA5CD56-30CC-4C38-A9B1-CB38FBF56566}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C1" sqref="C1:AF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>2019</v>
-      </c>
-      <c r="C1">
         <v>2020</v>
       </c>
-      <c r="D1">
-        <v>2021</v>
-      </c>
-      <c r="E1">
-        <v>2022</v>
-      </c>
-      <c r="F1">
-        <v>2023</v>
-      </c>
-      <c r="G1">
-        <v>2024</v>
-      </c>
-      <c r="H1">
-        <v>2025</v>
-      </c>
-      <c r="I1">
-        <v>2026</v>
-      </c>
-      <c r="J1">
-        <v>2027</v>
-      </c>
-      <c r="K1">
-        <v>2028</v>
-      </c>
-      <c r="L1">
-        <v>2029</v>
-      </c>
-      <c r="M1">
-        <v>2030</v>
-      </c>
-      <c r="N1">
-        <v>2031</v>
-      </c>
-      <c r="O1">
-        <v>2032</v>
-      </c>
-      <c r="P1">
-        <v>2033</v>
-      </c>
-      <c r="Q1">
-        <v>2034</v>
-      </c>
-      <c r="R1">
-        <v>2035</v>
-      </c>
-      <c r="S1">
-        <v>2036</v>
-      </c>
-      <c r="T1">
-        <v>2037</v>
-      </c>
-      <c r="U1">
-        <v>2038</v>
-      </c>
-      <c r="V1">
-        <v>2039</v>
-      </c>
-      <c r="W1">
-        <v>2040</v>
-      </c>
-      <c r="X1">
-        <v>2041</v>
-      </c>
-      <c r="Y1">
-        <v>2042</v>
-      </c>
-      <c r="Z1">
-        <v>2043</v>
-      </c>
-      <c r="AA1">
-        <v>2044</v>
-      </c>
-      <c r="AB1">
-        <v>2045</v>
-      </c>
-      <c r="AC1">
-        <v>2046</v>
-      </c>
-      <c r="AD1">
-        <v>2047</v>
-      </c>
-      <c r="AE1">
-        <v>2048</v>
-      </c>
-      <c r="AF1">
-        <v>2049</v>
-      </c>
-      <c r="AG1">
-        <v>2050</v>
-      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="10">
-        <f>Calculations!B6+Calculations!C17</f>
-        <v>2753809.5238095238</v>
-      </c>
-      <c r="C2" s="10">
         <f>Calculations!C6+Calculations!D17</f>
         <v>3244718.6147186132</v>
       </c>
-      <c r="D2" s="10">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="33" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>2021</v>
+      </c>
+      <c r="C1">
+        <v>2022</v>
+      </c>
+      <c r="D1">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2024</v>
+      </c>
+      <c r="F1">
+        <v>2025</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+      <c r="H1">
+        <v>2027</v>
+      </c>
+      <c r="I1">
+        <v>2028</v>
+      </c>
+      <c r="J1">
+        <v>2029</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1">
+        <v>2031</v>
+      </c>
+      <c r="M1">
+        <v>2032</v>
+      </c>
+      <c r="N1">
+        <v>2033</v>
+      </c>
+      <c r="O1">
+        <v>2034</v>
+      </c>
+      <c r="P1">
+        <v>2035</v>
+      </c>
+      <c r="Q1">
+        <v>2036</v>
+      </c>
+      <c r="R1">
+        <v>2037</v>
+      </c>
+      <c r="S1">
+        <v>2038</v>
+      </c>
+      <c r="T1">
+        <v>2039</v>
+      </c>
+      <c r="U1">
+        <v>2040</v>
+      </c>
+      <c r="V1">
+        <v>2041</v>
+      </c>
+      <c r="W1">
+        <v>2042</v>
+      </c>
+      <c r="X1">
+        <v>2043</v>
+      </c>
+      <c r="Y1">
+        <v>2044</v>
+      </c>
+      <c r="Z1">
+        <v>2045</v>
+      </c>
+      <c r="AA1">
+        <v>2046</v>
+      </c>
+      <c r="AB1">
+        <v>2047</v>
+      </c>
+      <c r="AC1">
+        <v>2048</v>
+      </c>
+      <c r="AD1">
+        <v>2049</v>
+      </c>
+      <c r="AE1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
         <f>Calculations!D6+Calculations!E17</f>
         <v>4022727.2727272725</v>
       </c>
-      <c r="E2" s="10">
+      <c r="C2" s="10">
         <f>Calculations!E6+Calculations!F17</f>
         <v>5061645.0216450226</v>
       </c>
-      <c r="F2" s="10">
+      <c r="D2" s="10">
         <f>Calculations!F6+Calculations!G17</f>
         <v>6361471.8614718635</v>
       </c>
-      <c r="G2" s="10">
+      <c r="E2" s="10">
         <f>Calculations!G6+Calculations!H17</f>
         <v>7922207.7922077961</v>
       </c>
-      <c r="H2" s="10">
+      <c r="F2" s="10">
         <f>Calculations!H6+Calculations!I17</f>
         <v>9743852.8138528112</v>
       </c>
-      <c r="I2" s="10">
+      <c r="G2" s="10">
         <f>Calculations!I6+Calculations!J17</f>
         <v>11883549.783549769</v>
       </c>
-      <c r="J2" s="10">
+      <c r="H2" s="10">
         <f>Calculations!J6+Calculations!K17</f>
         <v>14284155.844155841</v>
       </c>
-      <c r="K2" s="10">
+      <c r="I2" s="10">
         <f>Calculations!K6+Calculations!L17</f>
         <v>16945670.995671004</v>
       </c>
-      <c r="L2" s="10">
+      <c r="J2" s="10">
         <f>Calculations!L6+Calculations!M17</f>
         <v>19868095.238095224</v>
       </c>
-      <c r="M2" s="10">
+      <c r="K2" s="10">
         <f>Calculations!M6+Calculations!N17</f>
         <v>23051428.571428567</v>
       </c>
-      <c r="N2" s="10">
+      <c r="L2" s="10">
         <f>Calculations!N6+Calculations!O17</f>
         <v>26590504.883231863</v>
       </c>
-      <c r="O2" s="10">
+      <c r="M2" s="10">
         <f>Calculations!O6+Calculations!P17</f>
         <v>30451291.969841164</v>
       </c>
-      <c r="P2" s="10">
+      <c r="N2" s="10">
         <f>Calculations!P6+Calculations!Q17</f>
         <v>34625483.028302878</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="O2" s="10">
         <f>Calculations!Q6+Calculations!R17</f>
         <v>39100082.542929463</v>
       </c>
-      <c r="R2" s="10">
+      <c r="P2" s="10">
         <f>Calculations!R6+Calculations!S17</f>
         <v>43858202.807596385</v>
       </c>
-      <c r="S2" s="10">
+      <c r="Q2" s="10">
         <f>Calculations!S6+Calculations!T17</f>
         <v>48941924.928247198</v>
       </c>
-      <c r="T2" s="10">
+      <c r="R2" s="10">
         <f>Calculations!T6+Calculations!U17</f>
         <v>54267594.819736868</v>
       </c>
-      <c r="U2" s="10">
+      <c r="S2" s="10">
         <f>Calculations!U6+Calculations!V17</f>
         <v>59812507.056451716</v>
       </c>
-      <c r="V2" s="10">
+      <c r="T2" s="10">
         <f>Calculations!V6+Calculations!W17</f>
         <v>65553857.384140566</v>
       </c>
-      <c r="W2" s="10">
+      <c r="U2" s="10">
         <f>Calculations!W6+Calculations!X17</f>
         <v>71469444.314851895</v>
       </c>
-      <c r="X2" s="10">
+      <c r="V2" s="10">
         <f>Calculations!X6+Calculations!Y17</f>
         <v>77600103.236268982</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="W2" s="10">
         <f>Calculations!Y6+Calculations!Z17</f>
         <v>83864354.000003025</v>
       </c>
-      <c r="Z2" s="10">
+      <c r="X2" s="10">
         <f>Calculations!Z6+Calculations!AA17</f>
         <v>90244328.616034582</v>
       </c>
-      <c r="AA2" s="10">
+      <c r="Y2" s="10">
         <f>Calculations!AA6+Calculations!AB17</f>
         <v>96723957.862693533</v>
       </c>
-      <c r="AB2" s="10">
+      <c r="Z2" s="10">
         <f>Calculations!AB6+Calculations!AC17</f>
         <v>103288969.05164808</v>
       </c>
-      <c r="AC2" s="10">
+      <c r="AA2" s="10">
         <f>Calculations!AC6+Calculations!AD17</f>
         <v>109914912.1892807</v>
       </c>
-      <c r="AD2" s="10">
+      <c r="AB2" s="10">
         <f>Calculations!AD6+Calculations!AE17</f>
         <v>116602761.39532638</v>
       </c>
-      <c r="AE2" s="10">
+      <c r="AC2" s="10">
         <f>Calculations!AE6+Calculations!AF17</f>
         <v>123343062.49466863</v>
       </c>
-      <c r="AF2" s="10">
+      <c r="AD2" s="10">
         <f>Calculations!AF6+Calculations!AG17</f>
         <v>130127688.44581467</v>
       </c>
-      <c r="AG2" s="10">
+      <c r="AE2" s="10">
         <f>Calculations!AG6+Calculations!AH17</f>
         <v>136949688.84400424</v>
       </c>

</xml_diff>